<commit_message>
Upgraded to API 2.5
</commit_message>
<xml_diff>
--- a/documents/Published/Dynamic Tooltip/DynamicTooltipByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Dynamic Tooltip/DynamicTooltipByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitLab_PowerBIVisuals\documents\Published\Dynamic Tooltip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual\documents\Published\Dynamic Tooltip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E83897F-12A6-4E0F-8448-1E68803D41FA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D3C00B-A4AB-45F6-9DE5-01FCAA26B868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15285" windowHeight="4935" xr2:uid="{97DCB166-1937-475F-B7FA-86832FE14153}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{97DCB166-1937-475F-B7FA-86832FE14153}"/>
   </bookViews>
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>S no</t>
   </si>
@@ -231,6 +231,18 @@
     <t>1. Erase the values in 'Header' and leave it blank
 2. Erase the values in 'Body' and leave it blank
 3. Hover on the Visual</t>
+  </si>
+  <si>
+    <t>PowerBi Desktop</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>IE</t>
   </si>
 </sst>
 </file>
@@ -332,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -355,6 +367,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,6 +396,1419 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2000249</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1704975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{978304CB-CC43-4714-971C-153451E281D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11772900" y="257175"/>
+          <a:ext cx="1847849" cy="1638300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1841979</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1657349</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BE79013-4FA6-40BA-862B-2915F65AD375}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11887200" y="2600325"/>
+          <a:ext cx="1575279" cy="1523999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1933575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1425185</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{610B6024-CE2F-4CA3-A10B-CEA2854F9A7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11868150" y="4591051"/>
+          <a:ext cx="1685925" cy="1406134"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1962151</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1494367</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAD4C9C0-B317-4266-8093-50995216432E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11849101" y="6115050"/>
+          <a:ext cx="1733550" cy="1437217"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1885950</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1446906</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03C4929B-3075-40C3-846C-85698A8A656C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11858625" y="7800976"/>
+          <a:ext cx="1647825" cy="1380230"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1847851</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1331498</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92F2FA5E-A569-4F0E-85C3-9F1104278A77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11887201" y="9439276"/>
+          <a:ext cx="1581150" cy="1302922"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2028825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1647701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC8A182-8FC9-4D68-B3D9-2E5AA5A6D9BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11753850" y="10868025"/>
+          <a:ext cx="1895475" cy="1590551"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1752600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1414153</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3A7FE27-F6AD-4F01-BFCC-999A445A73C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11763375" y="12601575"/>
+          <a:ext cx="1609725" cy="1337953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1866900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1815587</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC962838-AE13-43F9-B520-683AD5DFFF36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14135100" y="238125"/>
+          <a:ext cx="1600200" cy="1767962"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1752600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1990183</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3950A04D-B716-4741-A400-DF030FEB9755}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14011275" y="2181226"/>
+          <a:ext cx="1609725" cy="1856832"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1457325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1475572</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30E1F839-DFBA-4426-B866-1C548A6B23D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14058900" y="4181476"/>
+          <a:ext cx="1266825" cy="1446996"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1575230</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1543051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F4AA738-BBDA-41E1-95AE-07B4A29DDDF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14163676" y="5715001"/>
+          <a:ext cx="1279954" cy="1466850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1876425</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1565079</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBF0E545-DA11-4B58-99D1-25A8D4CC22CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14144625" y="7391400"/>
+          <a:ext cx="1600200" cy="1488879"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1479080</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1314451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67548C0C-4DCD-45D9-8D79-9D3585566929}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14287500" y="9067801"/>
+          <a:ext cx="1059980" cy="1238250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1704975</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1645401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D73A656A-7552-487B-9720-87E9D51D596E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14249400" y="10496550"/>
+          <a:ext cx="1323975" cy="1540626"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1619250</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1495936</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2987EB6A-7FF6-436B-8D5D-E26FB61D9C17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14239875" y="12153900"/>
+          <a:ext cx="1247775" cy="1448311"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1621571</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1695450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CE5B805-35A0-4B3A-83CA-C98D9E1A571E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16144875" y="323850"/>
+          <a:ext cx="1450121" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1777268</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1962151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E51066D-2E74-48D8-B3AB-1335AB42B47E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16078200" y="2181226"/>
+          <a:ext cx="1672493" cy="1828800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1528742</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1438275</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{562D1AC5-A831-4AE8-90EC-313580661EB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16268700" y="4229100"/>
+          <a:ext cx="1233467" cy="1362075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1657350</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1641625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFD3E50F-BE74-4BBC-9D0B-C8C554903C02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16163925" y="5695951"/>
+          <a:ext cx="1466850" cy="1584474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1657351</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1605644</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24013548-3E84-4EEE-A1D2-D210C3EC1AED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16202026" y="7362826"/>
+          <a:ext cx="1428750" cy="1558018"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1498477</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1323975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{715DDE89-A8C3-4CE7-92CB-A087953D15E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16363950" y="9086851"/>
+          <a:ext cx="1107952" cy="1228724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219076</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1704976</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1691444</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDDC52EE-E7EF-40A4-ADAA-FA5198CBE066}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16192501" y="10458450"/>
+          <a:ext cx="1485900" cy="1624769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1485900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1445454</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0413134D-6BB7-4CC8-89C4-CCC70EA1303C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16202025" y="12172950"/>
+          <a:ext cx="1257300" cy="1378779"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1676400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1720329</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA3C355F-F291-47B7-9AEA-EE8EE01E9C88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18068925" y="285750"/>
+          <a:ext cx="1533525" cy="1625079"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1673327</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1809750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C31C9F6-123A-4503-A742-42761FA6B078}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18040350" y="2171700"/>
+          <a:ext cx="1559027" cy="1685925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>21587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1591019</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1448170</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38143B0F-22E5-4C5B-A2ED-494E7108C345}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18192750" y="4174487"/>
+          <a:ext cx="1324319" cy="1426583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1657351</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1604963</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEE0AB3F-4B4E-4FDC-9D48-A952743E82A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18116551" y="5676900"/>
+          <a:ext cx="1466850" cy="1566863"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1619250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1603570</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{114336DC-A12F-414B-9828-029D15101DE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18097500" y="7381875"/>
+          <a:ext cx="1447800" cy="1536895"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1666875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1396964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE725478-2B12-40F0-8EE7-68C6DBD9CE45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18107025" y="9039225"/>
+          <a:ext cx="1485900" cy="1349339"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1733550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1504638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83BF4E69-ED8F-4667-A268-B9A6896577A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18021300" y="10439400"/>
+          <a:ext cx="1638300" cy="1457013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1676401</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1360690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7582A87-32EB-49B8-AF3A-08D180EAE2C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18211801" y="12125325"/>
+          <a:ext cx="1390650" cy="1341640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -682,10 +2108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5956C572-3390-4C5B-816D-9D0DD3C60BEE}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,9 +2120,13 @@
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
     <col min="5" max="5" width="43.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -712,8 +2142,20 @@
       <c r="E1" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -730,7 +2172,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9" t="s">
@@ -743,7 +2185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
@@ -756,7 +2198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="132" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -767,7 +2209,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="132" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
@@ -780,7 +2222,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>2</v>
       </c>
@@ -797,7 +2239,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -814,10 +2256,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -829,6 +2271,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1029,7 +2472,7 @@
       <c r="B17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="11" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1038,14 +2481,14 @@
       <c r="B18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="11"/>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
@@ -1065,7 +2508,7 @@
       <c r="B21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1074,21 +2517,21 @@
       <c r="B22" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C22" s="13"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="13"/>
+      <c r="C24" s="14"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6">

</xml_diff>